<commit_message>
Integration test with excel file.
</commit_message>
<xml_diff>
--- a/tests/fixtures/basic.xlsx
+++ b/tests/fixtures/basic.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>id</t>
   </si>
@@ -25,6 +25,9 @@
     <t>language</t>
   </si>
   <si>
+    <t>notSupported</t>
+  </si>
+  <si>
     <t>John Doe</t>
   </si>
   <si>
@@ -41,6 +44,12 @@
   </si>
   <si>
     <t>fr</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>Extra</t>
   </si>
   <si>
     <t>Mary Doe</t>
@@ -132,10 +141,10 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1188,16 +1197,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="6.82031" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.0156" style="1" customWidth="1"/>
-    <col min="4" max="5" width="8.85156" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.85156" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6719" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85156" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.125" style="1" customWidth="1"/>
     <col min="6" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1214,100 +1224,115 @@
       <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
+      <c r="E1" t="s" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" s="4">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>6</v>
-      </c>
-      <c r="E2" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>9</v>
-      </c>
-      <c r="E3" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s" s="2">
-        <v>8</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" t="s" s="2">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s" s="2">
-        <v>13</v>
-      </c>
-      <c r="E5" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" ht="13.55" customHeight="1">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>